<commit_message>
code refactor - 1
</commit_message>
<xml_diff>
--- a/hackathon_data.xlsx
+++ b/hackathon_data.xlsx
@@ -461,22 +461,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>07 Mar 2023</t>
+          <t>28 Feb 2023</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> COGNIT '23 </t>
+          <t xml:space="preserve"> Smart Bengal Hackathon 2023 </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Technical, Symposium, Online, Hackathon</t>
+          <t>Technical, Hackathon</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>MNM Jain Engineering College</t>
+          <t>RCC Institute of Information Technology</t>
         </is>
       </c>
     </row>
@@ -486,22 +486,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>10 Mar 2023</t>
+          <t>07 Mar 2023</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ideathon 2023 </t>
+          <t xml:space="preserve"> COGNIT '23 </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Technical, Hackathon</t>
+          <t>Technical, Symposium, Online, Hackathon</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Francis Xavier Engineering College</t>
+          <t>MNM Jain Engineering College</t>
         </is>
       </c>
     </row>
@@ -516,17 +516,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> CONOCITHON 2.0 </t>
+          <t xml:space="preserve"> Ideathon 2023 </t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Online, Hackathon</t>
+          <t>Technical, Hackathon</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>St. Joseph's College of Engineering</t>
+          <t>Francis Xavier Engineering College</t>
         </is>
       </c>
     </row>
@@ -541,17 +541,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> GAMIGO-2023 </t>
+          <t xml:space="preserve"> CONOCITHON 2.0 </t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Hackathon</t>
+          <t>Online, Hackathon</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>K Ramakrishnan College of Engineering</t>
+          <t>St. Joseph's College of Engineering</t>
         </is>
       </c>
     </row>
@@ -561,22 +561,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>25 Feb 2023</t>
+          <t>10 Mar 2023</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> SRIT TECHNOVATION HACKATHON 2023 </t>
+          <t xml:space="preserve"> GAMIGO-2023 </t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Technical, Conference, Hackathon</t>
+          <t>Hackathon</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Sri Ramakrishna Institute of Technology</t>
+          <t>K Ramakrishnan College of Engineering</t>
         </is>
       </c>
     </row>
@@ -586,22 +586,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>10 Mar 2023</t>
+          <t>25 Feb 2023</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> TECHNO SYNC 2023 </t>
+          <t xml:space="preserve"> SRIT TECHNOVATION HACKATHON 2023 </t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Technical, Hackathon</t>
+          <t>Technical, Conference, Hackathon</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Karpagam College of Engineering</t>
+          <t>Sri Ramakrishna Institute of Technology</t>
         </is>
       </c>
     </row>
@@ -611,22 +611,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>28 Feb 2023</t>
+          <t>10 Mar 2023</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Skysprint Ideathon 2023 </t>
+          <t xml:space="preserve"> TECHNO SYNC 2023 </t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Webinar, Hackathon</t>
+          <t>Technical, Hackathon</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Kumaraguru College of Technology</t>
+          <t>Karpagam College of Engineering</t>
         </is>
       </c>
     </row>
@@ -636,22 +636,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>03 Mar 2023</t>
+          <t>28 Feb 2023</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Skara 23 </t>
+          <t xml:space="preserve"> Skysprint Ideathon 2023 </t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Technical, Symposium, Hackathon</t>
+          <t>Webinar, Hackathon</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>VSB Engineering College</t>
+          <t>Kumaraguru College of Technology</t>
         </is>
       </c>
     </row>
@@ -661,22 +661,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>06 Mar 2023</t>
+          <t>03 Mar 2023</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Femina Hack Fest 2023 </t>
+          <t xml:space="preserve"> Skara 23 </t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Hackathon</t>
+          <t>Technical, Symposium, Hackathon</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>KGiSL Institute of Technology</t>
+          <t>VSB Engineering College</t>
         </is>
       </c>
     </row>
@@ -686,22 +686,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>18 Feb 2023</t>
+          <t>06 Mar 2023</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ureckon 2023/ Product Game 2023 </t>
+          <t xml:space="preserve"> Femina Hack Fest 2023 </t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Management, Hackathon</t>
+          <t>Hackathon</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>University of Engineering and Management Kolkata</t>
+          <t>KGiSL Institute of Technology</t>
         </is>
       </c>
     </row>

</xml_diff>